<commit_message>
mengerjakan bayar beli paket data telkomsel negative, paket data xl positive dan negative (on progress)
</commit_message>
<xml_diff>
--- a/IOS/Bayar Beli - Pulsa dan Data Telkomsel/Default.xlsx
+++ b/IOS/Bayar Beli - Pulsa dan Data Telkomsel/Default.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="SpreadsheetGear 8.2.5.102"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
-    <sheet name="Pulsa Data Telkomsel - Positive" sheetId="2" r:id="rId2"/>
+    <sheet name="Paket Data Telkomsel - Positive" sheetId="2" r:id="rId2"/>
+    <sheet name="Paket Data Telkomsel - Negative" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
@@ -549,7 +550,7 @@
     <col min="7" max="16384" width="8.8984375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1">
+    <row r="1" ht="14.95" customFormat="1">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -594,7 +595,7 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -603,7 +604,26 @@
     <col min="1" max="16384" width="8.8984375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customFormat="1"/>
+    <row r="1" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[regresi] change profile pic, delete profile pic, change email positive dan negative, pulsa telkomsel positive(onprogress)
</commit_message>
<xml_diff>
--- a/IOS/Bayar Beli - Pulsa dan Data Telkomsel/Default.xlsx
+++ b/IOS/Bayar Beli - Pulsa dan Data Telkomsel/Default.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="SpreadsheetGear 8.2.5.102"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
     <sheet name="Paket Data Telkomsel - Positive" sheetId="2" r:id="rId2"/>
     <sheet name="Paket Data Telkomsel - Negative" sheetId="3" r:id="rId3"/>
+    <sheet name="Pulsa Telkomsel - Positive" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
@@ -614,7 +615,7 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -623,6 +624,25 @@
     <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" ht="14.95" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.95"/>
+  <cols>
+    <col min="1" max="16384" width="8.8984375" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
     <row r="1" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
pulsa telkomsel positive dan negative
</commit_message>
<xml_diff>
--- a/IOS/Bayar Beli - Pulsa dan Data Telkomsel/Default.xlsx
+++ b/IOS/Bayar Beli - Pulsa dan Data Telkomsel/Default.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="SpreadsheetGear 8.2.5.102"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
     <sheet name="Paket Data Telkomsel - Positive" sheetId="2" r:id="rId2"/>
     <sheet name="Paket Data Telkomsel - Negative" sheetId="3" r:id="rId3"/>
     <sheet name="Pulsa Telkomsel - Positive" sheetId="4" r:id="rId4"/>
+    <sheet name="Pulsa Telkomsel - Negative" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
@@ -634,7 +635,7 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -647,4 +648,23 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>